<commit_message>
Fixed excel files titls
</commit_message>
<xml_diff>
--- a/data/brief/briefP/Parents/b_2.0-3.11_gen.xlsx
+++ b/data/brief/briefP/Parents/b_2.0-3.11_gen.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\daniel\Documents\Daniel\My_projects\coding\Diagnostic_test\Diascore-backend\data\brief\briefP\Parents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127222E1-FA3E-4E22-B840-1FE69A8C63E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="4650" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -25,9 +31,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,6 +43,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -70,25 +81,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -99,10 +113,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -140,71 +154,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -232,7 +246,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -255,11 +269,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -268,13 +282,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -284,7 +298,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -293,7 +307,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -302,7 +316,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -310,10 +324,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -378,21 +392,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -400,7 +415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>189</v>
       </c>
@@ -408,7 +423,7 @@
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>188</v>
       </c>
@@ -416,7 +431,7 @@
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>187</v>
       </c>
@@ -424,7 +439,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>186</v>
       </c>
@@ -432,7 +447,7 @@
         <v>102</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>185</v>
       </c>
@@ -440,7 +455,7 @@
         <v>102</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>184</v>
       </c>
@@ -448,7 +463,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>183</v>
       </c>
@@ -456,7 +471,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>182</v>
       </c>
@@ -464,7 +479,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>181</v>
       </c>
@@ -472,7 +487,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>180</v>
       </c>
@@ -480,7 +495,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>179</v>
       </c>
@@ -488,7 +503,7 @@
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>178</v>
       </c>
@@ -496,7 +511,7 @@
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>177</v>
       </c>
@@ -504,7 +519,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>176</v>
       </c>
@@ -512,7 +527,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>175</v>
       </c>
@@ -520,7 +535,7 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>174</v>
       </c>
@@ -528,7 +543,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>173</v>
       </c>
@@ -536,7 +551,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>172</v>
       </c>
@@ -544,7 +559,7 @@
         <v>94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>171</v>
       </c>
@@ -552,7 +567,7 @@
         <v>94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>170</v>
       </c>
@@ -560,7 +575,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>169</v>
       </c>
@@ -568,7 +583,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>168</v>
       </c>
@@ -576,7 +591,7 @@
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>167</v>
       </c>
@@ -584,7 +599,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>166</v>
       </c>
@@ -592,7 +607,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>165</v>
       </c>
@@ -600,7 +615,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>164</v>
       </c>
@@ -608,7 +623,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>163</v>
       </c>
@@ -616,7 +631,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>162</v>
       </c>
@@ -624,7 +639,7 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>161</v>
       </c>
@@ -632,7 +647,7 @@
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>160</v>
       </c>
@@ -640,7 +655,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>159</v>
       </c>
@@ -648,7 +663,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>158</v>
       </c>
@@ -656,7 +671,7 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>157</v>
       </c>
@@ -664,7 +679,7 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>156</v>
       </c>
@@ -672,7 +687,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>155</v>
       </c>
@@ -680,7 +695,7 @@
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>154</v>
       </c>
@@ -688,7 +703,7 @@
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>153</v>
       </c>
@@ -696,7 +711,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>152</v>
       </c>
@@ -704,7 +719,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>151</v>
       </c>
@@ -712,7 +727,7 @@
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>150</v>
       </c>
@@ -720,7 +735,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>149</v>
       </c>
@@ -728,7 +743,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>148</v>
       </c>
@@ -736,7 +751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>147</v>
       </c>
@@ -744,7 +759,7 @@
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>146</v>
       </c>
@@ -752,7 +767,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>145</v>
       </c>
@@ -760,7 +775,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>144</v>
       </c>
@@ -768,7 +783,7 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>143</v>
       </c>
@@ -776,7 +791,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>142</v>
       </c>
@@ -784,7 +799,7 @@
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>141</v>
       </c>
@@ -792,7 +807,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>140</v>
       </c>
@@ -800,7 +815,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>139</v>
       </c>
@@ -808,7 +823,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>138</v>
       </c>
@@ -816,7 +831,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>137</v>
       </c>
@@ -824,7 +839,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>136</v>
       </c>
@@ -832,7 +847,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>135</v>
       </c>
@@ -840,7 +855,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>134</v>
       </c>
@@ -848,7 +863,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>133</v>
       </c>
@@ -856,7 +871,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>132</v>
       </c>
@@ -864,7 +879,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>131</v>
       </c>
@@ -872,7 +887,7 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>130</v>
       </c>
@@ -880,7 +895,7 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row r="62" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>129</v>
       </c>
@@ -888,7 +903,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row r="63" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>128</v>
       </c>
@@ -896,7 +911,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row r="64" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>127</v>
       </c>
@@ -904,7 +919,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row r="65" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>126</v>
       </c>
@@ -912,7 +927,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row r="66" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>125</v>
       </c>
@@ -920,7 +935,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row r="67" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>124</v>
       </c>
@@ -928,7 +943,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row r="68" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>123</v>
       </c>
@@ -936,7 +951,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row r="69" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>122</v>
       </c>
@@ -944,7 +959,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row r="70" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>121</v>
       </c>
@@ -952,7 +967,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row r="71" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>120</v>
       </c>
@@ -960,7 +975,7 @@
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row r="72" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>119</v>
       </c>
@@ -968,7 +983,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row r="73" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>118</v>
       </c>
@@ -976,7 +991,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row r="74" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>117</v>
       </c>
@@ -984,7 +999,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row r="75" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>116</v>
       </c>
@@ -992,7 +1007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row r="76" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>115</v>
       </c>
@@ -1000,7 +1015,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row r="77" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>114</v>
       </c>
@@ -1008,7 +1023,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row r="78" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>113</v>
       </c>
@@ -1016,7 +1031,7 @@
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row r="79" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>112</v>
       </c>
@@ -1024,7 +1039,7 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row r="80" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>111</v>
       </c>
@@ -1032,7 +1047,7 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row r="81" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>110</v>
       </c>
@@ -1040,7 +1055,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row r="82" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>109</v>
       </c>
@@ -1048,7 +1063,7 @@
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>108</v>
       </c>
@@ -1056,7 +1071,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>107</v>
       </c>
@@ -1064,7 +1079,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>106</v>
       </c>
@@ -1072,7 +1087,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>105</v>
       </c>
@@ -1080,7 +1095,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>104</v>
       </c>
@@ -1088,7 +1103,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>103</v>
       </c>
@@ -1096,7 +1111,7 @@
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>102</v>
       </c>
@@ -1104,7 +1119,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>101</v>
       </c>
@@ -1112,7 +1127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>100</v>
       </c>
@@ -1120,7 +1135,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>99</v>
       </c>
@@ -1128,7 +1143,7 @@
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>98</v>
       </c>
@@ -1136,7 +1151,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>97</v>
       </c>
@@ -1144,7 +1159,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>96</v>
       </c>
@@ -1152,7 +1167,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -1160,7 +1175,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>94</v>
       </c>
@@ -1168,7 +1183,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>93</v>
       </c>
@@ -1176,7 +1191,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>92</v>
       </c>
@@ -1184,7 +1199,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>91</v>
       </c>
@@ -1192,7 +1207,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>90</v>
       </c>
@@ -1200,7 +1215,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>89</v>
       </c>
@@ -1208,7 +1223,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>88</v>
       </c>
@@ -1216,7 +1231,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>87</v>
       </c>
@@ -1224,7 +1239,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>86</v>
       </c>
@@ -1232,7 +1247,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>85</v>
       </c>
@@ -1240,7 +1255,7 @@
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
+    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>84</v>
       </c>
@@ -1248,7 +1263,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>83</v>
       </c>
@@ -1256,7 +1271,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
+    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>82</v>
       </c>
@@ -1264,7 +1279,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>81</v>
       </c>
@@ -1272,7 +1287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>80</v>
       </c>
@@ -1280,7 +1295,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
+    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>79</v>
       </c>
@@ -1288,7 +1303,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
+    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>78</v>
       </c>
@@ -1296,7 +1311,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
+    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>77</v>
       </c>
@@ -1304,7 +1319,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
+    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>76</v>
       </c>
@@ -1312,7 +1327,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
+    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>75</v>
       </c>
@@ -1320,7 +1335,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
+    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>74</v>
       </c>
@@ -1328,7 +1343,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
+    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>73</v>
       </c>
@@ -1336,7 +1351,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
+    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>72</v>
       </c>
@@ -1344,7 +1359,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
+    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>71</v>
       </c>
@@ -1352,7 +1367,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
+    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>70</v>
       </c>
@@ -1360,7 +1375,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
+    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>69</v>
       </c>
@@ -1368,7 +1383,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
+    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>68</v>
       </c>
@@ -1376,7 +1391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
+    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>67</v>
       </c>
@@ -1384,7 +1399,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
+    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>66</v>
       </c>
@@ -1392,7 +1407,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
+    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>65</v>
       </c>
@@ -1400,7 +1415,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>64</v>
       </c>
@@ -1408,7 +1423,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>63</v>
       </c>

</xml_diff>